<commit_message>
update data and network aesthetics
</commit_message>
<xml_diff>
--- a/data/2019-22.xlsx
+++ b/data/2019-22.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/thesis/github/broomball/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA3C84D-1D58-F94F-9B44-815AC8380CC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918885C7-FAD7-594B-8F3C-98A3C5118018}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="4" r:id="rId1"/>
     <sheet name="roster" sheetId="3" r:id="rId2"/>
     <sheet name="1-1" sheetId="1" r:id="rId3"/>
     <sheet name="1-2" sheetId="2" r:id="rId4"/>
+    <sheet name="2-1" sheetId="5" r:id="rId5"/>
+    <sheet name="2-3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="114">
   <si>
     <t>team</t>
   </si>
@@ -346,13 +348,43 @@
   </si>
   <si>
     <t>call</t>
+  </si>
+  <si>
+    <t>2019-06-22</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>00:56</t>
+  </si>
+  <si>
+    <t>01:15</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>17:15</t>
+  </si>
+  <si>
+    <t>09:17</t>
+  </si>
+  <si>
+    <t>20:18</t>
+  </si>
+  <si>
+    <t>Roughing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -364,6 +396,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -386,12 +425,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -710,14 +752,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CCCB8-BB0F-4490-AE5B-B361C4570FB8}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -739,7 +781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -750,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -761,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -783,12 +825,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -802,7 +844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -816,7 +858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -830,7 +872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -844,7 +886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -858,7 +900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -872,7 +914,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -886,7 +928,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -900,7 +942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -914,7 +956,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -928,7 +970,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -942,7 +984,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -956,7 +998,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
@@ -973,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9C9460-99D3-024B-8457-83452005E34A}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1676,4 +1718,514 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30F1FD7-21AD-B144-884A-CFD11895EDA1}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB671153-EBC5-9541-B418-E889AC094DC8}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
typo 2-3 -> 2-2
</commit_message>
<xml_diff>
--- a/data/2019-22.xlsx
+++ b/data/2019-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/thesis/github/broomball/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918885C7-FAD7-594B-8F3C-98A3C5118018}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180ACAF1-F60C-704D-A58B-7AE89262F74C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="5" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="1-1" sheetId="1" r:id="rId3"/>
     <sheet name="1-2" sheetId="2" r:id="rId4"/>
     <sheet name="2-1" sheetId="5" r:id="rId5"/>
-    <sheet name="2-3" sheetId="6" r:id="rId6"/>
+    <sheet name="2-2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -752,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CCCB8-BB0F-4490-AE5B-B361C4570FB8}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1923,7 +1923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB671153-EBC5-9541-B418-E889AC094DC8}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
standings, data format addition
combined goalie and skater stats
adding match info to each game sheet to account for teams that didn't score
</commit_message>
<xml_diff>
--- a/data/2019-22.xlsx
+++ b/data/2019-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/thesis/github/broomball/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180ACAF1-F60C-704D-A58B-7AE89262F74C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE919705-9DD2-C649-B1D3-DE0AED5B7FF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="5" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="121">
   <si>
     <t>team</t>
   </si>
@@ -378,6 +378,27 @@
   </si>
   <si>
     <t>Roughing</t>
+  </si>
+  <si>
+    <t>Red Velvet Cake</t>
+  </si>
+  <si>
+    <t>Fighting Eeyores</t>
+  </si>
+  <si>
+    <t>The Suspencer is Killing Me</t>
+  </si>
+  <si>
+    <t>Sorcerer's Apparatus</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>away</t>
   </si>
 </sst>
 </file>
@@ -752,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89CCCB8-BB0F-4490-AE5B-B361C4570FB8}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -772,7 +793,7 @@
     </row>
     <row r="2" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -783,7 +804,7 @@
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -794,7 +815,7 @@
     </row>
     <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -805,7 +826,7 @@
     </row>
     <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -1013,7 +1034,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9C9460-99D3-024B-8457-83452005E34A}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1028,159 +1049,97 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>63</v>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>66</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1188,59 +1147,88 @@
         <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -1249,21 +1237,76 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1274,7 +1317,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA687585-D33A-9448-80D2-200385CAD219}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1285,159 +1328,97 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>84</v>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1445,28 +1426,28 @@
         <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>37</v>
+        <v>68</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1477,12 +1458,18 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1497,22 +1484,22 @@
         <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>72</v>
@@ -1523,22 +1510,28 @@
         <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1552,109 +1545,94 @@
         <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="H15" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>93</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1662,28 +1640,28 @@
         <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -1691,27 +1669,114 @@
         <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>96</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1722,7 +1787,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30F1FD7-21AD-B144-884A-CFD11895EDA1}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1733,184 +1798,206 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>84</v>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>72</v>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1921,9 +2008,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB671153-EBC5-9541-B418-E889AC094DC8}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1937,162 +2024,97 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>62</v>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2100,22 +2122,28 @@
         <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -2125,17 +2153,20 @@
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
-        <v>2</v>
+      <c r="C12" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>11</v>
+      <c r="F12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>62</v>
@@ -2144,84 +2175,162 @@
         <v>72</v>
       </c>
     </row>
+    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>96</v>
+        <v>40</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>62</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding week 3 games
</commit_message>
<xml_diff>
--- a/data/2019-22.xlsx
+++ b/data/2019-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m29605/Documents/thesis/github/broomball/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE919705-9DD2-C649-B1D3-DE0AED5B7FF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC47D55E-4E9D-1E4C-81E1-91E9FD6F3B39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{3D9C33C8-65AB-974C-BB77-375D6032BA6B}"/>
   </bookViews>
@@ -19,6 +19,8 @@
     <sheet name="1-2" sheetId="2" r:id="rId4"/>
     <sheet name="2-1" sheetId="5" r:id="rId5"/>
     <sheet name="2-2" sheetId="6" r:id="rId6"/>
+    <sheet name="3-1" sheetId="7" r:id="rId7"/>
+    <sheet name="3-2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="142">
   <si>
     <t>team</t>
   </si>
@@ -125,9 +127,6 @@
     <t>Dai Tran-Trong</t>
   </si>
   <si>
-    <t>Joe Nudi</t>
-  </si>
-  <si>
     <t>Nathan Centofanti</t>
   </si>
   <si>
@@ -200,12 +199,6 @@
     <t>meta</t>
   </si>
   <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -399,6 +392,78 @@
   </si>
   <si>
     <t>away</t>
+  </si>
+  <si>
+    <t>06/29/2019</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Joe Nudi III</t>
+  </si>
+  <si>
+    <t>16:45</t>
+  </si>
+  <si>
+    <t>12:20</t>
+  </si>
+  <si>
+    <t>07:50</t>
+  </si>
+  <si>
+    <t>14:15</t>
+  </si>
+  <si>
+    <t>08:38</t>
+  </si>
+  <si>
+    <t>06:20</t>
+  </si>
+  <si>
+    <t>03:46</t>
+  </si>
+  <si>
+    <t>02:25</t>
+  </si>
+  <si>
+    <t>10:40</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>12:10</t>
+  </si>
+  <si>
+    <t>02:48</t>
+  </si>
+  <si>
+    <t>01:37</t>
+  </si>
+  <si>
+    <t>14:01</t>
+  </si>
+  <si>
+    <t>13:47</t>
+  </si>
+  <si>
+    <t>07:36</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>verb</t>
+  </si>
+  <si>
+    <t>pulled</t>
+  </si>
+  <si>
+    <t>02:20</t>
   </si>
 </sst>
 </file>
@@ -446,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -456,6 +521,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,7 +861,7 @@
     </row>
     <row r="2" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -804,7 +872,7 @@
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -815,7 +883,7 @@
     </row>
     <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -826,7 +894,7 @@
     </row>
     <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -931,33 +999,33 @@
       <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
+      <c r="D6" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
@@ -965,66 +1033,66 @@
     </row>
     <row r="9" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1034,7 +1102,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9C9460-99D3-024B-8457-83452005E34A}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1049,18 +1117,21 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -1068,167 +1139,203 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>62</v>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>63</v>
+      <c r="D10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -1237,77 +1344,22 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>16</v>
+        <v>77</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" s="1" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1317,7 +1369,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA687585-D33A-9448-80D2-200385CAD219}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1328,18 +1380,21 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1347,437 +1402,418 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>63</v>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>84</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H15" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>4</v>
+        <v>73</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>93</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1823,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30F1FD7-21AD-B144-884A-CFD11895EDA1}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1798,18 +1834,21 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -1817,188 +1856,169 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>63</v>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>100</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2008,7 +2028,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB671153-EBC5-9541-B418-E889AC094DC8}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2024,18 +2044,21 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -2043,295 +2066,1074 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>85</v>
+      <c r="C12" s="1">
+        <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D57F14-7291-8047-B4A7-36F1DA33FCAF}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEC369-CB54-EB4E-BF0F-6662B3B760D9}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
     <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>81</v>
+      <c r="C20" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>